<commit_message>
Removecd all info not needed to be SimpleBox34pfas.
</commit_message>
<xml_diff>
--- a/SimpleBox4PFAS/src/main/webapp/resources/templates/nanomaterials.xlsx
+++ b/SimpleBox4PFAS/src/main/webapp/resources/templates/nanomaterials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\git\SimpleBox4PFAS\SimpleBox4PFAS\src\main\webapp\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B8437C-8CC2-48E3-8985-B529A9B28D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744166CF-4159-4034-9480-35B93E87F41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Nr</t>
   </si>
@@ -116,181 +116,16 @@
     <t>EF(soil)</t>
   </si>
   <si>
-    <t>RadS</t>
-  </si>
-  <si>
     <t>RhoS</t>
-  </si>
-  <si>
-    <t>AHamakerSP.w</t>
-  </si>
-  <si>
-    <t>AtefSA.w0</t>
-  </si>
-  <si>
-    <t>AtefSP.w0</t>
-  </si>
-  <si>
-    <t>AtefSA.w1</t>
-  </si>
-  <si>
-    <t>AtefSP.w1</t>
-  </si>
-  <si>
-    <t>AtefSA.w2</t>
-  </si>
-  <si>
-    <t>AtefSP.w2</t>
-  </si>
-  <si>
-    <t>AtefSA.w3</t>
-  </si>
-  <si>
-    <t>AtefSP.w3</t>
-  </si>
-  <si>
-    <t>AtefSA.s1</t>
-  </si>
-  <si>
-    <t>AtefSP.s1</t>
-  </si>
-  <si>
-    <t>AtefSA.s2</t>
-  </si>
-  <si>
-    <t>AtefSP.s2</t>
-  </si>
-  <si>
-    <t>AtefSA.s3</t>
-  </si>
-  <si>
-    <t>AtefSP.s3</t>
-  </si>
-  <si>
-    <t>AtefSA.sd0</t>
-  </si>
-  <si>
-    <t>AtefSP.sd0</t>
-  </si>
-  <si>
-    <t>AtefSA.sd1</t>
-  </si>
-  <si>
-    <t>AtefSP.sd1</t>
-  </si>
-  <si>
-    <t>AtefSA.sd2</t>
-  </si>
-  <si>
-    <t>AtefSP.sd2</t>
-  </si>
-  <si>
-    <t>kdis.w0S.w0D</t>
-  </si>
-  <si>
-    <t>kdis.w0A.w0D</t>
-  </si>
-  <si>
-    <t>kdis.w0P.w0D</t>
-  </si>
-  <si>
-    <t>kdis.w1S.w1D</t>
-  </si>
-  <si>
-    <t>kdis.w1A.w1D</t>
-  </si>
-  <si>
-    <t>kdis.w1P.w1D</t>
-  </si>
-  <si>
-    <t>kdis.w2S.w2D</t>
-  </si>
-  <si>
-    <t>kdis.w2A.w2D</t>
-  </si>
-  <si>
-    <t>kdis.w2P.w2D</t>
-  </si>
-  <si>
-    <t>kdis.s1S.s1D</t>
-  </si>
-  <si>
-    <t>kdis.s1A.s1D</t>
-  </si>
-  <si>
-    <t>kdis.s1P.s1D</t>
-  </si>
-  <si>
-    <t>kdis.s2S.s2D</t>
-  </si>
-  <si>
-    <t>kdis.s2A.s2D</t>
-  </si>
-  <si>
-    <t>kdis.s2P.s2D</t>
-  </si>
-  <si>
-    <t>kdis.s3S.s3D</t>
-  </si>
-  <si>
-    <t>kdis.s3A.s3D</t>
-  </si>
-  <si>
-    <t>kdis.s3P.s3D</t>
-  </si>
-  <si>
-    <t>kdis.sd0S.sd0D</t>
-  </si>
-  <si>
-    <t>kdis.sd0A.sd0D</t>
-  </si>
-  <si>
-    <t>kdis.sd0P.sd0D</t>
-  </si>
-  <si>
-    <t>kdis.sd1S.sd1D</t>
-  </si>
-  <si>
-    <t>kdis.sd1A.sd1D</t>
-  </si>
-  <si>
-    <t>kdis.sd1P.sd1D</t>
-  </si>
-  <si>
-    <t>kdis.sd2S.sd2D</t>
-  </si>
-  <si>
-    <t>kdis.sd2A.sd2D</t>
-  </si>
-  <si>
-    <t>kdis.sd2P.sd2D</t>
-  </si>
-  <si>
-    <t>kdis.w3S.w3D</t>
-  </si>
-  <si>
-    <t>kdis.w3A.w3D</t>
-  </si>
-  <si>
-    <t>kdis.w3P.w3D</t>
   </si>
   <si>
     <t>Pa</t>
   </si>
   <si>
-    <t>[nm]</t>
-  </si>
-  <si>
     <t>[kg.m-3]</t>
   </si>
   <si>
-    <t>[J]</t>
-  </si>
-  <si>
     <t>[-]</t>
-  </si>
-  <si>
-    <t>[s-1]</t>
   </si>
   <si>
     <t>nanoparticle</t>
@@ -323,15 +158,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>X3</t>
-  </si>
-  <si>
     <t>g.mol-1</t>
   </si>
   <si>
@@ -353,145 +179,10 @@
     <t>t.yr-1</t>
   </si>
   <si>
-    <t>kdegS.a</t>
-  </si>
-  <si>
-    <t>kfragS.a</t>
-  </si>
-  <si>
-    <t>kmpdeg.a</t>
-  </si>
-  <si>
-    <t>kdegS.w0</t>
-  </si>
-  <si>
-    <t>kdegS.w1</t>
-  </si>
-  <si>
-    <t>kfragS.w1</t>
-  </si>
-  <si>
-    <t>kmpdeg.w1</t>
-  </si>
-  <si>
-    <t>kdegS.w2</t>
-  </si>
-  <si>
-    <t>kfragS.w2</t>
-  </si>
-  <si>
-    <t>kmpdeg.w2</t>
-  </si>
-  <si>
-    <t>kdegS.s1</t>
-  </si>
-  <si>
-    <t>kdegS.s2</t>
-  </si>
-  <si>
-    <t>kdegS.s3</t>
-  </si>
-  <si>
-    <t>kfragS.s</t>
-  </si>
-  <si>
-    <t>kmpdeg.s</t>
-  </si>
-  <si>
-    <t>kdegS.sd0</t>
-  </si>
-  <si>
-    <t>kdegS.sd1</t>
-  </si>
-  <si>
-    <t>kdegS.sd2</t>
-  </si>
-  <si>
-    <t>kfragS.sd</t>
-  </si>
-  <si>
-    <t>kmpdeg.sd</t>
-  </si>
-  <si>
-    <t>kdegS.w3</t>
-  </si>
-  <si>
-    <t>kfragS.w3</t>
-  </si>
-  <si>
-    <t>kmpdeg.w3</t>
-  </si>
-  <si>
     <t>microplastic</t>
   </si>
   <si>
     <t>Particle</t>
-  </si>
-  <si>
-    <t>kdegA.a</t>
-  </si>
-  <si>
-    <t>kdegP.a</t>
-  </si>
-  <si>
-    <t>kdegA.w0</t>
-  </si>
-  <si>
-    <t>kdegP.w0</t>
-  </si>
-  <si>
-    <t>kdegA.w1</t>
-  </si>
-  <si>
-    <t>kdegP.w1</t>
-  </si>
-  <si>
-    <t>kdegA.w2</t>
-  </si>
-  <si>
-    <t>kdegP.w2</t>
-  </si>
-  <si>
-    <t>kdegA.s1</t>
-  </si>
-  <si>
-    <t>kdegP.s1</t>
-  </si>
-  <si>
-    <t>kdegA.s2</t>
-  </si>
-  <si>
-    <t>kdegP.s2</t>
-  </si>
-  <si>
-    <t>kdegA.s3</t>
-  </si>
-  <si>
-    <t>kdegP.s3</t>
-  </si>
-  <si>
-    <t>kdegA.sd0</t>
-  </si>
-  <si>
-    <t>kdegP.sd0</t>
-  </si>
-  <si>
-    <t>kdegA.sd1</t>
-  </si>
-  <si>
-    <t>kdegP.sd1</t>
-  </si>
-  <si>
-    <t>kdegA.sd2</t>
-  </si>
-  <si>
-    <t>kdegP.sd2</t>
-  </si>
-  <si>
-    <t>kdegA.w3</t>
-  </si>
-  <si>
-    <t>kdegP.w3</t>
   </si>
   <si>
     <t>PFAS</t>
@@ -505,7 +196,7 @@
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="General_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,15 +215,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,18 +237,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEAEAEA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -583,17 +261,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -605,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,9 +304,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -649,45 +313,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -697,10 +332,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -23534,8 +23166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ES12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BG16" sqref="BG16"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23561,807 +23193,189 @@
     <col min="24" max="24" width="9.6640625" style="7" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="12" style="8" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="9.33203125" style="8" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.5546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="4.44140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="9.21875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="8.5546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.44140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="51" width="9.21875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="57" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="9.21875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="11.77734375" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="62" width="11" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="78" width="9.21875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="79" width="12.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="80" max="80" width="11.88671875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="81" max="81" width="11.77734375" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="82" max="103" width="9.109375" style="9" collapsed="1"/>
-    <col min="104" max="104" width="10.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="105" max="115" width="9.109375" style="9"/>
-    <col min="116" max="126" width="9.109375" style="9" collapsed="1"/>
-    <col min="127" max="149" width="9.109375" style="9"/>
+    <col min="27" max="27" width="13.44140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="149" width="9.109375" style="9"/>
     <col min="150" max="16384" width="9.109375" style="9" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC1" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD1" s="17" t="s">
+      <c r="AA1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="I2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AU1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AZ1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="BB1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="BC1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BH1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="BI1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="BJ1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="BK1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="BL1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="BM1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="BN1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="BO1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP1" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="BQ1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="BR1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BS1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="BT1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="BU1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="BV1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="BX1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="BY1" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="BZ1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="CA1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="CB1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="CC1" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="CD1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="CE1" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="CF1" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="CG1" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="CH1" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="CI1" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="CJ1" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="CK1" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="CL1" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="CM1" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="CN1" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="CO1" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="CP1" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="CQ1" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="CR1" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="CS1" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="CT1" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="CU1" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="CV1" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="CW1" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="CX1" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="CY1" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="CZ1" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="DA1" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="DB1" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="DC1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="DD1" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="DE1" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="DF1" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="DG1" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="DH1" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="DI1" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="DJ1" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="DK1" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="DL1" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="DM1" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="DN1" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="DO1" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="DP1" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="DQ1" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="DR1" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="DS1" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="DT1" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="DU1" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="DV1" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="DW1" s="24" t="s">
-        <v>151</v>
-      </c>
     </row>
-    <row r="2" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD2" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AS2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AU2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AV2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AX2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AY2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BB2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BC2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BD2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BF2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BG2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BH2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BI2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BJ2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BK2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BL2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BM2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BN2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BP2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BQ2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BR2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BS2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BT2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BU2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BV2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BW2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BX2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BY2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BZ2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="CA2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="CB2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="CC2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="CD2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="CE2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CF2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CG2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CI2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CJ2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CK2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CL2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CM2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CN2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CO2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CP2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CQ2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CR2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CS2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CT2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CU2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CV2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CW2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CX2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CY2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="CZ2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DA2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DB2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DC2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DD2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DE2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DF2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DG2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DH2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DI2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DJ2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DK2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DL2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DM2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DN2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DO2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DP2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DQ2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DR2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DS2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DT2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DU2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DV2" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="DW2" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E3" s="9">
         <v>0</v>
@@ -24429,322 +23443,22 @@
       <c r="Z3" s="9">
         <v>0</v>
       </c>
-      <c r="AA3" s="9">
-        <v>6</v>
-      </c>
-      <c r="AB3" s="9">
-        <v>6</v>
-      </c>
-      <c r="AC3" s="9">
+      <c r="AA3" s="10">
         <v>0</v>
       </c>
-      <c r="AD3" s="18">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="11">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BA3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BC3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BD3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BE3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BF3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BG3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BH3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BJ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BK3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BL3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BM3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BN3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BO3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BP3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BQ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BR3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BS3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BT3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BU3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BV3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BW3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BX3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BY3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BZ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="CA3" s="9">
-        <v>0</v>
-      </c>
-      <c r="CB3" s="9">
-        <v>0</v>
-      </c>
-      <c r="CC3" s="9">
-        <v>0</v>
-      </c>
-      <c r="CD3" s="9">
-        <v>0</v>
-      </c>
-      <c r="CE3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY3" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV3" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW3" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>11</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E4" s="9">
         <v>0</v>
@@ -24812,322 +23526,22 @@
       <c r="Z4" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AA4" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="9">
-        <v>11</v>
-      </c>
-      <c r="AC4" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="18">
-        <v>75</v>
-      </c>
-      <c r="AE4" s="10">
+      <c r="AA4" s="10">
         <v>4230</v>
       </c>
-      <c r="AF4" s="11">
-        <v>1.9999999999999999E-20</v>
-      </c>
-      <c r="AG4" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AH4" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AI4" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AJ4" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AK4" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AP4" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AQ4" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AR4" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AS4" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AT4" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AU4" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AV4" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AW4" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AX4" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AY4" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ4" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BB4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BD4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BF4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BG4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BH4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BJ4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BK4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BM4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BN4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BO4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BQ4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BR4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BS4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BT4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BU4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BV4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BW4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BX4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BY4" s="9">
-        <v>0</v>
-      </c>
-      <c r="BZ4" s="9">
-        <v>0</v>
-      </c>
-      <c r="CA4" s="9">
-        <v>0</v>
-      </c>
-      <c r="CB4" s="9">
-        <v>0</v>
-      </c>
-      <c r="CC4" s="9">
-        <v>0</v>
-      </c>
-      <c r="CD4" s="9">
-        <v>0</v>
-      </c>
-      <c r="CE4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY4" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV4" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW4" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="C5" s="9">
         <v>0</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E5" s="9">
         <v>0</v>
@@ -25196,321 +23610,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AA5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="9">
-        <v>11</v>
-      </c>
-      <c r="AC5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="18">
-        <v>9.5</v>
-      </c>
-      <c r="AE5" s="9">
         <v>4230</v>
       </c>
-      <c r="AF5" s="9">
-        <v>6.9000000000000004E-21</v>
-      </c>
-      <c r="AG5" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="AH5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="AJ5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AK5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AP5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AR5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AT5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AU5" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="AV5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AW5" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="AX5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AY5" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="AZ5" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BB5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BG5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BH5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BL5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BM5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BN5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BO5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BP5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BQ5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BR5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BS5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BT5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BU5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BV5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BW5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BX5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BY5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BZ5" s="9">
-        <v>0</v>
-      </c>
-      <c r="CA5" s="9">
-        <v>0</v>
-      </c>
-      <c r="CB5" s="9">
-        <v>0</v>
-      </c>
-      <c r="CC5" s="9">
-        <v>0</v>
-      </c>
-      <c r="CD5" s="9">
-        <v>0</v>
-      </c>
-      <c r="CE5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY5" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV5" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW5" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>13</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E6" s="9">
         <v>0</v>
@@ -25579,321 +23693,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AA6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="9">
-        <v>13</v>
-      </c>
-      <c r="AC6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="18">
-        <v>75</v>
-      </c>
-      <c r="AE6" s="9">
         <v>10500</v>
       </c>
-      <c r="AF6" s="9">
-        <v>2.02E-20</v>
-      </c>
-      <c r="AG6" s="9">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="AH6" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AI6" s="9">
-        <v>0.38</v>
-      </c>
-      <c r="AJ6" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AK6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO6" s="9">
-        <v>0.08</v>
-      </c>
-      <c r="AP6" s="9">
-        <v>0.08</v>
-      </c>
-      <c r="AQ6" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="AR6" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="AS6" s="9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AT6" s="9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AU6" s="9">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="AV6" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AW6" s="9">
-        <v>0.38</v>
-      </c>
-      <c r="AX6" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AY6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ6" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BB6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BC6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BD6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BE6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BF6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BG6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BH6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BI6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BJ6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BK6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BL6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BM6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BN6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BO6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BP6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BQ6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BR6" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BS6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BT6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BU6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BV6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BW6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BX6" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BY6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BZ6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CA6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CB6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CC6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CD6" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CE6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY6" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV6" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW6" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E7" s="9">
         <v>0</v>
@@ -25962,321 +23776,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AA7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="9">
-        <v>14</v>
-      </c>
-      <c r="AC7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="18">
-        <v>75</v>
-      </c>
-      <c r="AE7" s="9">
         <v>5610</v>
       </c>
-      <c r="AF7" s="9">
-        <v>1.6900000000000001E-20</v>
-      </c>
-      <c r="AG7" s="9">
-        <v>0.62</v>
-      </c>
-      <c r="AH7" s="9">
-        <v>0.26</v>
-      </c>
-      <c r="AI7" s="9">
-        <v>0.62</v>
-      </c>
-      <c r="AJ7" s="9">
-        <v>0.26</v>
-      </c>
-      <c r="AK7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO7" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="AP7" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="AQ7" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="AR7" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="AS7" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="AT7" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="AU7" s="9">
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="AV7" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="AW7" s="9">
-        <v>3.5999999999999998E-6</v>
-      </c>
-      <c r="AX7" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="AY7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ7" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BB7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BC7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BD7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BE7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BF7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BG7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BH7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BI7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="BJ7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BK7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BL7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BM7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BN7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BO7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BP7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BQ7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BR7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BS7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BT7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BU7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BV7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BW7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BX7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BY7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="BZ7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="CA7" s="25">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="CB7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="CC7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="CD7" s="9">
-        <v>1.6500000000000001E-6</v>
-      </c>
-      <c r="CE7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY7" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV7" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW7" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E8" s="9">
         <v>0</v>
@@ -26345,321 +23859,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AA8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="9">
-        <v>8</v>
-      </c>
-      <c r="AC8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="18">
-        <v>5</v>
-      </c>
-      <c r="AE8" s="9">
         <v>1650</v>
       </c>
-      <c r="AF8" s="9">
-        <v>2.7600000000000001E-20</v>
-      </c>
-      <c r="AG8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AH8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AI8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AJ8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AK8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO8" s="9">
-        <v>0.1022</v>
-      </c>
-      <c r="AP8" s="9">
-        <v>0.1022</v>
-      </c>
-      <c r="AQ8" s="9">
-        <v>0.1022</v>
-      </c>
-      <c r="AR8" s="9">
-        <v>0.1022</v>
-      </c>
-      <c r="AS8" s="9">
-        <v>0.1022</v>
-      </c>
-      <c r="AT8" s="9">
-        <v>0.1022</v>
-      </c>
-      <c r="AU8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AV8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AW8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AX8" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="AY8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ8" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BB8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BC8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BE8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BH8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BI8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BK8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BM8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BN8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BO8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BQ8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BR8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BS8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BT8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BU8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BV8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BW8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BX8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BY8" s="9">
-        <v>0</v>
-      </c>
-      <c r="BZ8" s="9">
-        <v>0</v>
-      </c>
-      <c r="CA8" s="9">
-        <v>0</v>
-      </c>
-      <c r="CB8" s="9">
-        <v>0</v>
-      </c>
-      <c r="CC8" s="9">
-        <v>0</v>
-      </c>
-      <c r="CD8" s="9">
-        <v>0</v>
-      </c>
-      <c r="CE8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY8" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV8" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW8" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>9</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E9" s="9">
         <v>0</v>
@@ -26728,321 +23942,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AA9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="9">
-        <v>9</v>
-      </c>
-      <c r="AC9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="18">
-        <v>5</v>
-      </c>
-      <c r="AE9" s="9">
         <v>10500</v>
       </c>
-      <c r="AF9" s="9">
-        <v>2.02E-20</v>
-      </c>
-      <c r="AG9" s="9">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="AH9" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AI9" s="9">
-        <v>0.38</v>
-      </c>
-      <c r="AJ9" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AK9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO9" s="9">
-        <v>0.08</v>
-      </c>
-      <c r="AP9" s="9">
-        <v>0.08</v>
-      </c>
-      <c r="AQ9" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="AR9" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="AS9" s="9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AT9" s="9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AU9" s="9">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="AV9" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AW9" s="9">
-        <v>0.38</v>
-      </c>
-      <c r="AX9" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="AY9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ9" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BB9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BC9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BD9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BE9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BF9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BG9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BH9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BI9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BJ9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BK9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BL9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BM9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BN9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BO9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BP9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BQ9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BR9" s="9">
-        <v>4.87E-6</v>
-      </c>
-      <c r="BS9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BT9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BU9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BV9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BW9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BX9" s="9">
-        <v>1.3199999999999999E-7</v>
-      </c>
-      <c r="BY9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="BZ9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CA9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CB9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CC9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CD9" s="9">
-        <v>1.1800000000000001E-5</v>
-      </c>
-      <c r="CE9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY9" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV9" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW9" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
@@ -27111,321 +24025,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AA10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="9">
-        <v>10</v>
-      </c>
-      <c r="AC10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="19">
-        <v>5</v>
-      </c>
-      <c r="AE10" s="9">
         <v>4230</v>
       </c>
-      <c r="AF10" s="9">
-        <v>6.9000000000000004E-21</v>
-      </c>
-      <c r="AG10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AH10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AI10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AJ10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AK10" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM10" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN10" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO10" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AP10" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AQ10" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AR10" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AS10" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AT10" s="9">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="AU10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AV10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AW10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AX10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="AY10" s="9">
-        <v>1</v>
-      </c>
-      <c r="AZ10" s="9">
-        <v>1</v>
-      </c>
-      <c r="BA10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BB10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BC10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BD10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BE10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BF10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BG10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BH10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BI10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BJ10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BK10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BL10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BM10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BN10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BO10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BP10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BQ10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BR10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BS10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BT10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BU10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BV10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BW10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BX10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BY10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="BZ10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="CA10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="CB10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="CC10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="CD10" s="9">
-        <v>1E-13</v>
-      </c>
-      <c r="CE10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CF10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CG10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CH10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CI10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CJ10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CK10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CL10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CM10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CN10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CO10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CP10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CQ10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CR10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CS10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CT10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CU10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CV10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CW10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CX10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CY10" s="16">
-        <v>0</v>
-      </c>
-      <c r="CZ10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DA10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DB10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DC10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DD10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DE10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DF10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DG10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DH10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DI10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DJ10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DK10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DL10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DM10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DN10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DO10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DP10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DQ10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DR10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DS10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DT10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DU10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DV10" s="16">
-        <v>0</v>
-      </c>
-      <c r="DW10" s="16">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:127" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>128</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -27493,371 +24107,70 @@
       <c r="Z11" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="1">
-        <v>10</v>
-      </c>
-      <c r="AC11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="20">
-        <v>10</v>
-      </c>
-      <c r="AE11" s="20">
+      <c r="AA11" s="14">
         <f>4.23*10^3</f>
         <v>4230</v>
       </c>
-      <c r="AF11" s="21">
-        <f>6.9*10^-21</f>
-        <v>6.9000000000000004E-21</v>
-      </c>
-      <c r="AG11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AH11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AI11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AJ11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AK11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AP11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AQ11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AR11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AS11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AT11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AU11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AV11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AW11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AX11" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="AY11" s="21">
-        <v>1</v>
-      </c>
-      <c r="AZ11" s="22">
-        <v>1</v>
-      </c>
-      <c r="BA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CQ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CS11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CW11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CX11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CY11" s="1">
-        <v>0</v>
-      </c>
-      <c r="CZ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DE11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DF11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DH11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DI11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DJ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DK11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DL11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DM11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DN11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DO11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DP11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DQ11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DR11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DS11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DT11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DU11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DV11" s="1">
-        <v>0</v>
-      </c>
-      <c r="DW11" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:127" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="E12" s="3">
         <v>0.04</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="15">
         <v>214</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="15">
         <v>255</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="16">
         <v>851</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="16">
         <v>447</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="18">
         <v>1</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="18">
         <v>1</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="18">
         <v>1</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="18">
         <v>126000</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="18">
         <v>500</v>
       </c>
-      <c r="O12" s="29">
+      <c r="O12" s="18">
         <v>12600</v>
       </c>
-      <c r="P12" s="29">
+      <c r="P12" s="18">
         <v>950</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="Q12" s="17">
         <v>3.5007433361613397E-6</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12" s="17">
         <v>3.5007433361613399E-7</v>
       </c>
-      <c r="S12" s="28">
+      <c r="S12" s="17">
         <v>3.5007433361613399E-8</v>
       </c>
-      <c r="T12" s="28">
+      <c r="T12" s="17">
         <v>1.1325934322874922E-7</v>
       </c>
       <c r="U12" s="1">
@@ -27878,323 +24191,18 @@
       <c r="Z12" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AA12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="1">
-        <v>10</v>
-      </c>
-      <c r="AC12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL12" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN12" s="9">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AW12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AY12" s="20">
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BA12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BB12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BC12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BF12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BG12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BH12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BI12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BK12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BL12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BM12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BN12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BO12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BQ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BR12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BS12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BT12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BU12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BV12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BW12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BX12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BY12" s="20">
-        <v>0</v>
-      </c>
-      <c r="BZ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CA12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CB12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CC12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CD12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CE12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CF12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CG12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CH12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CI12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CJ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CK12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CL12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CM12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CN12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CO12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CP12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CQ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CR12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CS12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CT12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CU12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CV12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CW12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CX12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CY12" s="20">
-        <v>0</v>
-      </c>
-      <c r="CZ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DA12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DB12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DC12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DD12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DE12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DF12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DG12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DH12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DI12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DJ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DK12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DL12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DM12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DN12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DO12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DP12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DQ12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DR12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DS12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DT12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DU12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DV12" s="20">
-        <v>0</v>
-      </c>
-      <c r="DW12" s="20">
+      <c r="AA12" s="14">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E13:Z1048576 AB13:AB1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="E13:Z1048576">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:AC12">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BA11:DW11">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="E1:Z12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated nanomaterials. Fixed issue when changing MW.
</commit_message>
<xml_diff>
--- a/SimpleBox4PFAS/src/main/webapp/resources/templates/nanomaterials.xlsx
+++ b/SimpleBox4PFAS/src/main/webapp/resources/templates/nanomaterials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\git\SimpleBox4PFAS\SimpleBox4PFAS\src\main\webapp\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1542342-FDF1-485C-BCA5-663DC7E38990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4866DF-5796-4CA4-8FCC-958E5875025B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>Nr</t>
   </si>
@@ -205,14 +216,64 @@
   <si>
     <t>2706-90-3</t>
   </si>
+  <si>
+    <t>Acetic acid</t>
+  </si>
+  <si>
+    <t>64-19-7</t>
+  </si>
+  <si>
+    <t>PFAS alternative</t>
+  </si>
+  <si>
+    <t>60.06</t>
+  </si>
+  <si>
+    <t>Hexadecyltrimethoxysilane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16415-12-6
+</t>
+  </si>
+  <si>
+    <t>Trimethoxy(octyl)silane</t>
+  </si>
+  <si>
+    <t>3069-40-7</t>
+  </si>
+  <si>
+    <t>Hexamethyldisiloxane</t>
+  </si>
+  <si>
+    <t>107-46-0</t>
+  </si>
+  <si>
+    <t>1185-55-3</t>
+  </si>
+  <si>
+    <t>Trimethoxyphenylsilane</t>
+  </si>
+  <si>
+    <t>Trimethoxymethylsilane</t>
+  </si>
+  <si>
+    <t>2996-92-1</t>
+  </si>
+  <si>
+    <t>2-Octenylsuccinic Anhydride</t>
+  </si>
+  <si>
+    <t>42482-06-4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="General_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -276,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,6 +379,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -23156,10 +23220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ES14"/>
+  <dimension ref="A1:ES21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23167,10 +23231,10 @@
     <col min="1" max="1" width="5.88671875" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="31.44140625" style="9" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.33203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="5" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11.77734375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="7.21875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="11" width="8.109375" style="4" customWidth="1" collapsed="1"/>
@@ -24135,52 +24199,52 @@
       <c r="J12" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="1">
         <v>0</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="1">
         <v>0</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="1">
         <v>0</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="1">
         <v>0</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="1">
         <v>0</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="1">
         <v>0</v>
       </c>
-      <c r="Q12" s="11">
+      <c r="Q12" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="R12" s="11">
+      <c r="R12" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="S12" s="11">
+      <c r="S12" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="T12" s="11">
+      <c r="T12" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="U12" s="15">
+      <c r="U12" s="1">
         <v>0</v>
       </c>
-      <c r="V12" s="15">
+      <c r="V12" s="1">
         <v>0</v>
       </c>
-      <c r="W12" s="11">
+      <c r="W12" s="9">
         <v>30000</v>
       </c>
-      <c r="X12" s="11">
+      <c r="X12" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y12" s="11">
+      <c r="Y12" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z12" s="11">
+      <c r="Z12" s="9">
         <v>0.33333333333333331</v>
       </c>
       <c r="AA12" s="14">
@@ -24218,52 +24282,52 @@
       <c r="J13" s="4">
         <v>6.0999999999999997E-4</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="1">
         <v>0</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="1">
         <v>0</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="1">
         <v>0</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="1">
         <v>0</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="1">
         <v>0</v>
       </c>
-      <c r="P13" s="15">
+      <c r="P13" s="1">
         <v>0</v>
       </c>
-      <c r="Q13" s="11">
+      <c r="Q13" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="S13" s="11">
+      <c r="S13" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="T13" s="11">
+      <c r="T13" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="U13" s="15">
+      <c r="U13" s="1">
         <v>0</v>
       </c>
-      <c r="V13" s="15">
+      <c r="V13" s="1">
         <v>0</v>
       </c>
-      <c r="W13" s="11">
+      <c r="W13" s="9">
         <v>30000</v>
       </c>
-      <c r="X13" s="11">
+      <c r="X13" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y13" s="11">
+      <c r="Y13" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z13" s="11">
+      <c r="Z13" s="9">
         <v>0.33333333333333331</v>
       </c>
       <c r="AA13" s="14">
@@ -24301,56 +24365,637 @@
       <c r="J14" s="4">
         <v>10.5</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="1">
         <v>0</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="1">
         <v>0</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="1">
         <v>0</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="1">
         <v>0</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O14" s="1">
         <v>0</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="1">
         <v>0</v>
       </c>
-      <c r="Q14" s="11">
+      <c r="Q14" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="S14" s="11">
+      <c r="S14" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="T14" s="11">
+      <c r="T14" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U14" s="1">
         <v>0</v>
       </c>
-      <c r="V14" s="15">
+      <c r="V14" s="1">
         <v>0</v>
       </c>
-      <c r="W14" s="11">
+      <c r="W14" s="9">
         <v>30000</v>
       </c>
-      <c r="X14" s="11">
+      <c r="X14" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y14" s="11">
+      <c r="Y14" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z14" s="11">
+      <c r="Z14" s="9">
         <v>0.33333333333333331</v>
       </c>
       <c r="AA14" s="9">
         <v>1810</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>17</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="3">
+        <v>16.64</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2079</v>
+      </c>
+      <c r="I15" s="4">
+        <v>602.9</v>
+      </c>
+      <c r="J15" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-0.17</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R15" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S15" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T15" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U15" s="16">
+        <v>0</v>
+      </c>
+      <c r="V15" s="16">
+        <v>0</v>
+      </c>
+      <c r="W15" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X15" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y15" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z15" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>1044.5999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>18</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>346.62</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="J16" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K16" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R16" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S16" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T16" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U16" s="16">
+        <v>0</v>
+      </c>
+      <c r="V16" s="16">
+        <v>0</v>
+      </c>
+      <c r="W16" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X16" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y16" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z16" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA16" s="14">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>19</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>234.41</v>
+      </c>
+      <c r="G17" s="15">
+        <v>-66</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>13.3</v>
+      </c>
+      <c r="J17" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K17" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="L17" s="16">
+        <v>0</v>
+      </c>
+      <c r="M17" s="16">
+        <v>0</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0</v>
+      </c>
+      <c r="P17" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R17" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S17" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T17" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U17" s="16">
+        <v>0</v>
+      </c>
+      <c r="V17" s="16">
+        <v>0</v>
+      </c>
+      <c r="W17" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X17" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y17" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z17" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA17" s="9">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>20</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>162.38</v>
+      </c>
+      <c r="G18" s="15">
+        <v>-59</v>
+      </c>
+      <c r="H18" s="4">
+        <v>44000</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.93</v>
+      </c>
+      <c r="J18" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K18" s="4">
+        <v>4</v>
+      </c>
+      <c r="L18" s="16">
+        <v>0</v>
+      </c>
+      <c r="M18" s="16">
+        <v>0</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R18" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S18" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T18" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U18" s="16">
+        <v>0</v>
+      </c>
+      <c r="V18" s="16">
+        <v>0</v>
+      </c>
+      <c r="W18" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X18" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y18" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z18" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>763.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>21</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>136.22</v>
+      </c>
+      <c r="G19" s="15">
+        <v>-77</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1990</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="J19" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0</v>
+      </c>
+      <c r="M19" s="16">
+        <v>0</v>
+      </c>
+      <c r="N19" s="16">
+        <v>0</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0</v>
+      </c>
+      <c r="P19" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R19" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S19" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T19" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U19" s="16">
+        <v>0</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0</v>
+      </c>
+      <c r="W19" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X19" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y19" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z19" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA19" s="9">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>22</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>198.29</v>
+      </c>
+      <c r="G20" s="15">
+        <v>-25</v>
+      </c>
+      <c r="H20" s="4">
+        <v>12790</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1700</v>
+      </c>
+      <c r="J20" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K20" s="4">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R20" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S20" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T20" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U20" s="16">
+        <v>0</v>
+      </c>
+      <c r="V20" s="16">
+        <v>0</v>
+      </c>
+      <c r="W20" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X20" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y20" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z20" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA20" s="9">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>23</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>210.27</v>
+      </c>
+      <c r="G21" s="15">
+        <v>14.3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>43.5</v>
+      </c>
+      <c r="I21" s="4">
+        <v>20</v>
+      </c>
+      <c r="J21" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="K21" s="4">
+        <v>4.68</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0</v>
+      </c>
+      <c r="P21" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="R21" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="S21" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="T21" s="11">
+        <v>9.9999999999999995E-21</v>
+      </c>
+      <c r="U21" s="16">
+        <v>0</v>
+      </c>
+      <c r="V21" s="16">
+        <v>0</v>
+      </c>
+      <c r="W21" s="11">
+        <v>30000</v>
+      </c>
+      <c r="X21" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Y21" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z21" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Trimethoxy(octyl)silane properties in nanomaterials excel.
</commit_message>
<xml_diff>
--- a/SimpleBox4PFAS/src/main/webapp/resources/templates/nanomaterials.xlsx
+++ b/SimpleBox4PFAS/src/main/webapp/resources/templates/nanomaterials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\git\SimpleBox4PFAS\SimpleBox4PFAS\src\main\webapp\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7757C5-25D5-4897-92FE-EB3678D5ECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E419A47-CAF9-4F11-9626-3690557CB964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,17 +30,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -270,12 +259,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="General_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +290,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -337,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,26 +383,20 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -23235,10 +23225,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:ES21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23249,11 +23240,12 @@
     <col min="4" max="4" width="13.77734375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="5" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.77734375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11.77734375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="7.21875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="11" width="8.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="16" width="8" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="16" width="8" style="4" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="8.88671875" style="4" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="12" style="4" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="10" style="4" customWidth="1" collapsed="1"/>
@@ -24445,8 +24437,8 @@
       <c r="D15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="12">
-        <v>0</v>
+      <c r="E15" s="18">
+        <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>59</v>
@@ -24460,39 +24452,24 @@
       <c r="I15" s="4">
         <v>602.9</v>
       </c>
-      <c r="J15" s="11">
-        <v>9.9999999999999995E-21</v>
+      <c r="J15" s="19">
+        <v>0.19207109292930871</v>
       </c>
       <c r="K15" s="4">
-        <v>-0.17</v>
-      </c>
-      <c r="L15" s="16">
-        <v>0</v>
-      </c>
-      <c r="M15" s="16">
-        <v>0</v>
-      </c>
-      <c r="N15" s="16">
-        <v>0</v>
-      </c>
-      <c r="O15" s="16">
-        <v>0</v>
-      </c>
-      <c r="P15" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R15" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S15" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T15" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <f>10^(-0.17)</f>
+        <v>0.67608297539198181</v>
+      </c>
+      <c r="L15" s="17">
+        <v>8.2625916625981718E-2</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
       <c r="U15" s="16">
         <v>0</v>
       </c>
@@ -24528,8 +24505,8 @@
       <c r="D16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="12">
-        <v>0</v>
+      <c r="E16" s="18">
+        <v>7</v>
       </c>
       <c r="F16" s="3">
         <v>346.62</v>
@@ -24543,39 +24520,24 @@
       <c r="I16" s="4">
         <v>2E-3</v>
       </c>
-      <c r="J16" s="11">
-        <v>9.9999999999999995E-21</v>
+      <c r="J16" s="19">
+        <v>0.13990309867886785</v>
       </c>
       <c r="K16" s="4">
-        <v>8.1</v>
+        <f>10^8.1</f>
+        <v>125892541.17941682</v>
       </c>
       <c r="L16" s="17">
-        <v>1</v>
-      </c>
-      <c r="M16" s="17">
-        <v>126000</v>
-      </c>
-      <c r="N16" s="17">
-        <v>500</v>
-      </c>
-      <c r="O16" s="17">
-        <v>12600</v>
-      </c>
-      <c r="P16" s="17">
-        <v>950</v>
-      </c>
-      <c r="Q16" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R16" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S16" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T16" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <v>229266.47276014092</v>
+      </c>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="16">
         <v>0</v>
       </c>
@@ -24611,8 +24573,8 @@
       <c r="D17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="12">
-        <v>0</v>
+      <c r="E17" s="18">
+        <v>7</v>
       </c>
       <c r="F17" s="3">
         <v>234.41</v>
@@ -24620,45 +24582,30 @@
       <c r="G17" s="15">
         <v>-66</v>
       </c>
-      <c r="H17" s="4">
-        <v>0</v>
+      <c r="H17" s="9">
+        <v>2.4084152589004067E-36</v>
       </c>
       <c r="I17" s="4">
         <v>13.3</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="19">
         <v>9.9999999999999995E-21</v>
       </c>
       <c r="K17" s="4">
-        <v>3.9</v>
-      </c>
-      <c r="L17" s="16">
-        <v>0</v>
-      </c>
-      <c r="M17" s="16">
-        <v>0</v>
-      </c>
-      <c r="N17" s="16">
-        <v>0</v>
-      </c>
-      <c r="O17" s="16">
-        <v>0</v>
-      </c>
-      <c r="P17" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R17" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S17" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T17" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <f>10^3.9</f>
+        <v>7943.2823472428154</v>
+      </c>
+      <c r="L17" s="17">
+        <v>90.853267146066756</v>
+      </c>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
       <c r="U17" s="16">
         <v>0</v>
       </c>
@@ -24694,8 +24641,8 @@
       <c r="D18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="12">
-        <v>0</v>
+      <c r="E18" s="18">
+        <v>7</v>
       </c>
       <c r="F18" s="3">
         <v>162.38</v>
@@ -24709,39 +24656,24 @@
       <c r="I18" s="4">
         <v>0.93</v>
       </c>
-      <c r="J18" s="11">
-        <v>9.9999999999999995E-21</v>
+      <c r="J18" s="19">
+        <v>3100.8158889654519</v>
       </c>
       <c r="K18" s="4">
-        <v>4</v>
-      </c>
-      <c r="L18" s="16">
-        <v>0</v>
-      </c>
-      <c r="M18" s="16">
-        <v>0</v>
-      </c>
-      <c r="N18" s="16">
-        <v>0</v>
-      </c>
-      <c r="O18" s="16">
-        <v>0</v>
-      </c>
-      <c r="P18" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R18" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S18" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T18" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <f>10^4</f>
+        <v>10000</v>
+      </c>
+      <c r="L18" s="17">
+        <v>109.48145221121077</v>
+      </c>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
       <c r="U18" s="16">
         <v>0</v>
       </c>
@@ -24777,8 +24709,8 @@
       <c r="D19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="12">
-        <v>0</v>
+      <c r="E19" s="18">
+        <v>7</v>
       </c>
       <c r="F19" s="3">
         <v>136.22</v>
@@ -24792,39 +24724,24 @@
       <c r="I19" s="4">
         <v>1000000</v>
       </c>
-      <c r="J19" s="11">
-        <v>9.9999999999999995E-21</v>
+      <c r="J19" s="19">
+        <v>1.0941268306228841E-4</v>
       </c>
       <c r="K19" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="L19" s="16">
-        <v>0</v>
-      </c>
-      <c r="M19" s="16">
-        <v>0</v>
-      </c>
-      <c r="N19" s="16">
-        <v>0</v>
-      </c>
-      <c r="O19" s="16">
-        <v>0</v>
-      </c>
-      <c r="P19" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R19" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S19" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T19" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <f>10^0.7</f>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="L19" s="17">
+        <v>0.23245588709919471</v>
+      </c>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
       <c r="U19" s="16">
         <v>0</v>
       </c>
@@ -24860,8 +24777,8 @@
       <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="12">
-        <v>0</v>
+      <c r="E20" s="18">
+        <v>7</v>
       </c>
       <c r="F20" s="3">
         <v>198.29</v>
@@ -24875,39 +24792,24 @@
       <c r="I20" s="4">
         <v>1700</v>
       </c>
-      <c r="J20" s="11">
-        <v>9.9999999999999995E-21</v>
+      <c r="J20" s="19">
+        <v>0.60213816069071791</v>
       </c>
       <c r="K20" s="4">
-        <v>-2.1000000000000001E-2</v>
-      </c>
-      <c r="L20" s="16">
-        <v>0</v>
-      </c>
-      <c r="M20" s="16">
-        <v>0</v>
-      </c>
-      <c r="N20" s="16">
-        <v>0</v>
-      </c>
-      <c r="O20" s="16">
-        <v>0</v>
-      </c>
-      <c r="P20" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R20" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S20" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T20" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <f>10^-0.021</f>
+        <v>0.95279616402365186</v>
+      </c>
+      <c r="L20" s="17">
+        <v>6.0580178611949219E-2</v>
+      </c>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
       <c r="U20" s="16">
         <v>0</v>
       </c>
@@ -24943,8 +24845,8 @@
       <c r="D21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="12">
-        <v>0</v>
+      <c r="E21" s="18">
+        <v>7</v>
       </c>
       <c r="F21" s="3">
         <v>210.27</v>
@@ -24958,39 +24860,24 @@
       <c r="I21" s="4">
         <v>20</v>
       </c>
-      <c r="J21" s="11">
-        <v>9.9999999999999995E-21</v>
+      <c r="J21" s="19">
+        <v>0.18459090189911737</v>
       </c>
       <c r="K21" s="4">
-        <v>4.68</v>
-      </c>
-      <c r="L21" s="16">
-        <v>0</v>
-      </c>
-      <c r="M21" s="16">
-        <v>0</v>
-      </c>
-      <c r="N21" s="16">
-        <v>0</v>
-      </c>
-      <c r="O21" s="16">
-        <v>0</v>
-      </c>
-      <c r="P21" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="R21" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="S21" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="T21" s="11">
-        <v>9.9999999999999995E-21</v>
-      </c>
+        <f>10^4.68</f>
+        <v>47863.009232263823</v>
+      </c>
+      <c r="L21" s="17">
+        <v>389.17107091265768</v>
+      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="16">
         <v>0</v>
       </c>
@@ -25014,17 +24901,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:Z15 E17:Z1048576 E16:I16 U16:Z16">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16:K16 Q16:T16">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L16:P16">
+  <conditionalFormatting sqref="E1:Z1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>